<commit_message>
Update Topic 3 Slides
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kylebutts/Desktop/3535/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDF6C2C-87F3-8F47-90BB-BEA58FFD78D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D88D49C7-3667-1446-8539-AC427221D4BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="27160" xr2:uid="{8A5BAA71-3AF9-1A4B-A544-96432C83B05F}"/>
+    <workbookView xWindow="5640" yWindow="3000" windowWidth="51200" windowHeight="27160" xr2:uid="{8A5BAA71-3AF9-1A4B-A544-96432C83B05F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -299,7 +299,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -314,9 +314,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -344,16 +341,13 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -673,7 +667,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:XFD18"/>
+      <selection activeCell="C12" activeCellId="1" sqref="D11:E12 C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="16" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -681,6 +675,7 @@
     <col min="1" max="1" width="8.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="43.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" hidden="1"/>
   </cols>
   <sheetData>
@@ -708,9 +703,9 @@
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="8" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="7" t="s">
         <v>46</v>
       </c>
     </row>
@@ -721,11 +716,11 @@
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="9" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>23</v>
       </c>
     </row>
@@ -736,13 +731,13 @@
       <c r="B4" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="8" t="s">
         <v>26</v>
       </c>
     </row>
@@ -753,13 +748,13 @@
       <c r="B5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="8" t="s">
         <v>29</v>
       </c>
     </row>
@@ -770,13 +765,13 @@
       <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>32</v>
       </c>
     </row>
@@ -790,8 +785,8 @@
       <c r="C7" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="11" t="s">
+      <c r="D7" s="6"/>
+      <c r="E7" s="10" t="s">
         <v>47</v>
       </c>
     </row>
@@ -802,13 +797,13 @@
       <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="12" t="s">
+      <c r="E8" s="11" t="s">
         <v>36</v>
       </c>
     </row>
@@ -819,13 +814,13 @@
       <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="11" t="s">
         <v>39</v>
       </c>
     </row>
@@ -836,15 +831,13 @@
       <c r="B10" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="13" t="s">
-        <v>48</v>
-      </c>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
@@ -853,14 +846,12 @@
       <c r="B11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="6"/>
+      <c r="D11" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>42</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -870,14 +861,14 @@
       <c r="B12" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>45</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -887,15 +878,13 @@
       <c r="B13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="17" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>52</v>
-      </c>
+      <c r="C13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="6"/>
     </row>
     <row r="14" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
@@ -904,14 +893,14 @@
       <c r="B14" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="D14" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="17" t="s">
-        <v>55</v>
+      <c r="C14" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -921,14 +910,14 @@
       <c r="B15" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="D15" s="18" t="s">
-        <v>57</v>
-      </c>
-      <c r="E15" s="18" t="s">
-        <v>58</v>
+      <c r="C15" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
@@ -938,9 +927,15 @@
       <c r="B16" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="19"/>
+      <c r="C16" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="17" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
@@ -949,12 +944,11 @@
       <c r="B17" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
-    </row>
-    <row r="18" spans="1:5" s="16" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="16" t="s">
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+    </row>
+    <row r="18" spans="1:5" s="17" customFormat="1" ht="74" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="17" t="s">
         <v>21</v>
       </c>
     </row>

</xml_diff>